<commit_message>
added stuff to data plan
</commit_message>
<xml_diff>
--- a/planning/data_plan.xlsx
+++ b/planning/data_plan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>Data Plan</t>
   </si>
@@ -95,28 +95,127 @@
     <t>sign up / login</t>
   </si>
   <si>
+    <t>Allows users to create and log into their accounts</t>
+  </si>
+  <si>
+    <t>User-provided login credentials (email/username and password)</t>
+  </si>
+  <si>
+    <t>Check if the user's credentials match with the database. If yes, grant access to the user's account.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST request to </t>
+  </si>
+  <si>
     <t>manage user info</t>
   </si>
   <si>
+    <t>Allows users to manage their personal information</t>
+  </si>
+  <si>
+    <t>User-provided updated information (name, email, profile picture, etc.)</t>
+  </si>
+  <si>
+    <t>Update the user's information in the database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PUT request to </t>
+  </si>
+  <si>
     <t>join clubs</t>
   </si>
   <si>
-    <t>view updates</t>
+    <t>Allows users to join a club</t>
+  </si>
+  <si>
+    <t>Club ID of the club the user wants to join</t>
+  </si>
+  <si>
+    <t>Update the user's membership status in the club's database</t>
+  </si>
+  <si>
+    <t>view club updates</t>
+  </si>
+  <si>
+    <t>Allows users to view updates from the clubs they are members of</t>
+  </si>
+  <si>
+    <t>User ID of the user who wants to view the updates</t>
+  </si>
+  <si>
+    <t>Retrieve the updates from the club's database and filter them based on the user's membership status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GET request to </t>
   </si>
   <si>
     <t>view events / RSVP</t>
   </si>
   <si>
+    <t>Allows users to view upcoming club events and RSVP</t>
+  </si>
+  <si>
+    <t>User ID of the user who wants to view the events</t>
+  </si>
+  <si>
+    <t>Retrieve the events from the club's database and filter them based on the user's membership status. Update the user's RSVP status in the database if they choose to RSVP.</t>
+  </si>
+  <si>
+    <t>GET or PUT request to</t>
+  </si>
+  <si>
     <t>post updates</t>
   </si>
   <si>
+    <t>Allows club managers to post updates to their club's page</t>
+  </si>
+  <si>
+    <t>Club ID of the club the update is being posted to, update content</t>
+  </si>
+  <si>
+    <t>Add the update to the club's database</t>
+  </si>
+  <si>
     <t>create and update events</t>
   </si>
   <si>
+    <t xml:space="preserve"> Allows club managers to create and update club events</t>
+  </si>
+  <si>
+    <t>Club ID of the club the event is being created/updated for, event information</t>
+  </si>
+  <si>
+    <t>Add or update the event in the club's database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST or PUT request to </t>
+  </si>
+  <si>
     <t>view rsvps</t>
   </si>
   <si>
+    <t>Allows club managers to view who has RSVP'd for an event</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RSVP database.</t>
+  </si>
+  <si>
+    <t>Verify the identity and permissions of the user making the request.</t>
+  </si>
+  <si>
+    <t>GET request to</t>
+  </si>
+  <si>
     <t>email notifications</t>
+  </si>
+  <si>
+    <t>o allow users to sign up for email notifications from clubs for updates and special events, and to allow users to choose which types of notifications they receive for each club.</t>
+  </si>
+  <si>
+    <t>User input.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POST/PUT/DELETE request to </t>
   </si>
 </sst>
 </file>
@@ -632,12 +731,12 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="12" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="45.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="34.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="12" width="143.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="12" width="64.14785714285713" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="12" width="61.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="40.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="61.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="23.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="12" width="143.4335714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="12" width="76.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="12" width="55.29071428571429" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="12" width="45.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -721,108 +820,180 @@
       <c r="A5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="9"/>
-      <c r="G5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H5" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="F6" s="9"/>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="H6" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="F7" s="9"/>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H7" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="F8" s="9"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="H8" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>40</v>
+      </c>
       <c r="F9" s="9"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="H9" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
+        <v>42</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>44</v>
+      </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>45</v>
+      </c>
       <c r="F10" s="9"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>48</v>
+      </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="H11" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
+        <v>51</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>53</v>
+      </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="F12" s="9"/>
-      <c r="G12" s="8"/>
+      <c r="G12" s="8" t="s">
+        <v>55</v>
+      </c>
       <c r="H12" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
+        <v>56</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="F13" s="9"/>
-      <c r="G13" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>59</v>
+      </c>
       <c r="H13" s="8"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">

</xml_diff>

<commit_message>
adding files data plan and cap schema
</commit_message>
<xml_diff>
--- a/planning/data_plan.xlsx
+++ b/planning/data_plan.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="70">
   <si>
     <t>Data Plan</t>
   </si>
   <si>
-    <t>BITL_PT_2  Dylan Bui a1823679, Easwar Allada a1851456, Konstantinos Papagiannis a1825285 Nathaniel Cordero a1855786</t>
+    <t>Group Name/Number: UG061</t>
   </si>
   <si>
     <t>Feature/Interaction</t>
@@ -41,7 +41,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -51,7 +51,7 @@
       <rPr>
         <b/>
         <sz val="10"/>
-        <color theme="1"/>
+        <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
@@ -68,30 +68,6 @@
     <t>Other Notes</t>
   </si>
   <si>
-    <t>Restaurant Search</t>
-  </si>
-  <si>
-    <t>This is an example of an entry in a data plan for a restaurant booking system.&amp;#10;Users can search for restaurants and have the most relevant search results displayed.</t>
-  </si>
-  <si>
-    <t>A search bar/text input on the main search page</t>
-  </si>
-  <si>
-    <t>JSON formatted AJAX request containing the search term:&amp;#10;{ &amp;#10;    "query": "[the search bar contents]"&amp;#10;}</t>
-  </si>
-  <si>
-    <t>Find all restaurants in database whose names, locations, or cuisines match the search term.</t>
-  </si>
-  <si>
-    <t>JSON formatted AJAX response containing the the restaurant details:&amp;#10;[&amp;#10;    { &amp;#10;        "id": "restaurant id",&amp;#10;        "name": "restaurant name",&amp;#10;        "location": "restaurant location",&amp;#10;        "rating": "restaurant rating"&amp;#10;    },&amp;#10;    ...&amp;#10;]</t>
-  </si>
-  <si>
-    <t>POST Request&amp;#10;/restaurants</t>
-  </si>
-  <si>
-    <t>This same request could be achieved with a GET request via URL parameters, so when writing these yourself use your discretion.&amp;#10;By using a POST request with JSON body we can easily expand to additional fields like location or date range.</t>
-  </si>
-  <si>
     <t>sign up / login</t>
   </si>
   <si>
@@ -101,12 +77,21 @@
     <t>User-provided login credentials (email/username and password)</t>
   </si>
   <si>
+    <t>JSON formatted AJAX request containing the user login credentials:&amp;#10;{ &amp;#10;    "email": "[the user's email]"&amp;#10;    "password": "[the user's password]"&amp;#10;}</t>
+  </si>
+  <si>
     <t>Check if the user's credentials match with the database. If yes, grant access to the user's account.</t>
   </si>
   <si>
+    <t>JSON formatted AJAX response containing the login details:&amp;#10;[&amp;#10;    { &amp;#10;        "name": "user name",&amp;#10;        "login": "login successful"&amp;#10;    },&amp;#10;    ...&amp;#10;]</t>
+  </si>
+  <si>
     <t xml:space="preserve">POST request to </t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>manage user info</t>
   </si>
   <si>
@@ -116,9 +101,15 @@
     <t>User-provided updated information (name, email, profile picture, etc.)</t>
   </si>
   <si>
+    <t>JSON formatted AJAX request containing the user details:&amp;#10;{ &amp;#10;    "name": "[the user's name]"&amp;#10;    "email": "[the user's email]"&amp;#10;    "profile picture": "[the user's profile picture]"&amp;#10;}</t>
+  </si>
+  <si>
     <t>Update the user's information in the database</t>
   </si>
   <si>
+    <t>JSON formatted AJAX response containing the the restaurant details:&amp;#10;[&amp;#10;    { &amp;#10;        "name": "user name",&amp;#10;        "email": "user email",&amp;#10;        "profile picture": "user profile picture",&amp;#10;},&amp;#10;    ...&amp;#10;]</t>
+  </si>
+  <si>
     <t xml:space="preserve">PUT request to </t>
   </si>
   <si>
@@ -131,9 +122,15 @@
     <t>Club ID of the club the user wants to join</t>
   </si>
   <si>
+    <t>JSON formatted AJAX request containing the club ID and user ID:&amp;#10;{ &amp;#10;    "club ID": "[the club ID]"&amp;#10;    "user ID": "[the user ID]"&amp;#10;}</t>
+  </si>
+  <si>
     <t>Update the user's membership status in the club's database</t>
   </si>
   <si>
+    <t>JSON formatted AJAX response containing the membership details:&amp;#10;[&amp;#10;    { &amp;#10;        "membership": "membership type",&amp;#10;       },&amp;#10;    ...&amp;#10;]</t>
+  </si>
+  <si>
     <t>view club updates</t>
   </si>
   <si>
@@ -146,6 +143,9 @@
     <t>Retrieve the updates from the club's database and filter them based on the user's membership status</t>
   </si>
   <si>
+    <t>JSON formatted AJAX response containing the club updates:&amp;#10;[&amp;#10;    { &amp;#10;        "name": "club name",&amp;#10;        "logo": "club logo",&amp;#10;        "description": "club desc"&amp;#10;    },&amp;#10;    ...&amp;#10;]</t>
+  </si>
+  <si>
     <t xml:space="preserve">GET request to </t>
   </si>
   <si>
@@ -158,9 +158,15 @@
     <t>User ID of the user who wants to view the events</t>
   </si>
   <si>
+    <t>JSON formatted AJAX request containing the user ID:&amp;#10;{ &amp;#10;    "user ID": "[the user ID]"&amp;#10;}</t>
+  </si>
+  <si>
     <t>Retrieve the events from the club's database and filter them based on the user's membership status. Update the user's RSVP status in the database if they choose to RSVP.</t>
   </si>
   <si>
+    <t>JSON formatted AJAX response containing the upcoming events:&amp;#10;[&amp;#10;    { &amp;#10;        "events": "club upcoming events",&amp;#10;     },&amp;#10;    ...&amp;#10;]</t>
+  </si>
+  <si>
     <t>GET or PUT request to</t>
   </si>
   <si>
@@ -173,9 +179,15 @@
     <t>Club ID of the club the update is being posted to, update content</t>
   </si>
   <si>
+    <t>JSON formatted AJAX request containing the club ID:&amp;#10;{ &amp;#10;    "club ID": "[the club ID]"&amp;#10;}</t>
+  </si>
+  <si>
     <t>Add the update to the club's database</t>
   </si>
   <si>
+    <t>JSON formatted AJAX response containing the post details:&amp;#10;[&amp;#10;    { &amp;#10;        "post": "club post",&amp;#10;        "title": "post title",&amp;#10;        "content": "post content",&amp;#10;     },&amp;#10;    ...&amp;#10;]</t>
+  </si>
+  <si>
     <t>create and update events</t>
   </si>
   <si>
@@ -185,9 +197,16 @@
     <t>Club ID of the club the event is being created/updated for, event information</t>
   </si>
   <si>
+    <t xml:space="preserve">JSON formatted AJAX request containing the club ID:&amp;#10;{ &amp;#10;    "club ID": "[the club ID]"&amp;#10;}
+</t>
+  </si>
+  <si>
     <t>Add or update the event in the club's database</t>
   </si>
   <si>
+    <t>JSON formatted AJAX response containing the event details:&amp;#10;[&amp;#10;    { &amp;#10;        "event": "event id",&amp;#10;        "name": "event name",&amp;#10;        "location": "event location",&amp;#10;        "date": "event date"&amp;#10;        "description": "event desc",&amp;#10;    },&amp;#10;    ...&amp;#10;]</t>
+  </si>
+  <si>
     <t xml:space="preserve">POST or PUT request to </t>
   </si>
   <si>
@@ -197,22 +216,34 @@
     <t>Allows club managers to view who has RSVP'd for an event</t>
   </si>
   <si>
-    <t xml:space="preserve"> RSVP database.</t>
+    <t>User membership type</t>
+  </si>
+  <si>
+    <t>JSON formatted AJAX request containing the membership type of the user:&amp;#10;{ &amp;#10;    "membership type": "[the user's membership type]"&amp;#10;}</t>
   </si>
   <si>
     <t>Verify the identity and permissions of the user making the request.</t>
   </si>
   <si>
+    <t>JSON formatted AJAX response containing the RSVP details:&amp;#10;[&amp;#10;    { &amp;#10;        "names": "rsvp member names",&amp;#10;    },&amp;#10;    ...&amp;#10;]</t>
+  </si>
+  <si>
     <t>GET request to</t>
   </si>
   <si>
     <t>email notifications</t>
   </si>
   <si>
-    <t>o allow users to sign up for email notifications from clubs for updates and special events, and to allow users to choose which types of notifications they receive for each club.</t>
+    <t>Allow users to sign up for email notifications from clubs for updates and special events, and to allow users to choose which types of notifications they receive for each club.</t>
   </si>
   <si>
     <t>User input.</t>
+  </si>
+  <si>
+    <t>JSON formatted AJAX request containing the user choices:&amp;#10;{ &amp;#10;        "notifications": "[the user's input]"&amp;#10;}</t>
+  </si>
+  <si>
+    <t>JSON formatted AJAX response containing the updated notification settings:&amp;#10;[&amp;#10;    { &amp;#10;        "notifications": "user's notification choice",&amp;#10;    },&amp;#10;    ...&amp;#10;]</t>
   </si>
   <si>
     <t xml:space="preserve">POST/PUT/DELETE request to </t>
@@ -234,43 +265,43 @@
     <font>
       <b/>
       <sz val="24"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF2f4f4f"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF2f4f4f"/>
-      <name val="Monospace"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Monospace"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -280,11 +311,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFffffff"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFdcdcdc"/>
       </patternFill>
     </fill>
   </fills>
@@ -327,6 +353,13 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -338,21 +371,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFdcdcdc"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFdcdcdc"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFc6c6c6"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFc6c6c6"/>
       </bottom>
       <diagonal/>
     </border>
@@ -384,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -395,17 +413,20 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="5" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -420,7 +441,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,14 +751,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="12" width="26.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="12" width="143.57642857142858" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="12" width="64.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="61.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="143.4335714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="12" width="76.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="12" width="55.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="12" width="45.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="13" width="26.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="13" width="143.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="13" width="64.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="13" width="73.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="13" width="143.4335714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="13" width="76.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="13" width="55.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="13" width="45.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="33">
@@ -764,7 +785,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -790,7 +811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="120">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="118.5">
       <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
@@ -800,691 +821,727 @@
       <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>15</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="8" t="s">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="120.75">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="H5" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="107.25">
+      <c r="A6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="8" t="s">
+      <c r="B6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="G6" s="8" t="s">
+      <c r="C6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="8" t="s">
+      <c r="D6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="E6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="F6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8" t="s">
+      <c r="G6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="85.5">
+      <c r="A7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="8" t="s">
+      <c r="F7" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="9"/>
-      <c r="G8" s="8" t="s">
+      <c r="G7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
-      <c r="A9" s="8" t="s">
+      <c r="H7" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="110.25">
+      <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="8" t="s">
+      <c r="D8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="8" t="s">
+      <c r="E8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="8" t="s">
+      <c r="F8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="G8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="H8" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="118.5">
+      <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="8" t="s">
+      <c r="B9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="E9" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="9"/>
-      <c r="E11" s="8" t="s">
+      <c r="F9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="8" t="s">
+      <c r="G9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="34.5">
+      <c r="A10" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H11" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="8" t="s">
+      <c r="B10" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="8" t="s">
+      <c r="E10" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="8" t="s">
+      <c r="F10" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="8" t="s">
+      <c r="G10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="H10" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="130.5">
+      <c r="A11" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="B11" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="8" t="s">
+      <c r="C11" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="H13" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
+      <c r="D11" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="86.25">
+      <c r="A12" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H12" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="87">
+      <c r="A13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
-      <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
+      <c r="A30" s="6"/>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
-      <c r="A31" s="8"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="9"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="19.5">
-      <c r="A36" s="8"/>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="8"/>
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="19.5">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="9"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="9"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="19.5">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="9"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="9"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="9"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="9"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="8"/>
-      <c r="F49" s="9"/>
-      <c r="G49" s="8"/>
-      <c r="H49" s="8"/>
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="9"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="10"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
+      <c r="A52" s="9"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-      <c r="C53" s="8"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="9"/>
-      <c r="G53" s="8"/>
-      <c r="H53" s="8"/>
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="9"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="9"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="10"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
-      <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="8"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="8"/>
-      <c r="H58" s="8"/>
+      <c r="A58" s="9"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="10"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
+      <c r="A61" s="9"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="9"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
-      <c r="A62" s="10"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="11"/>
-      <c r="E62" s="10"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="10"/>
-      <c r="H62" s="10"/>
+      <c r="A62" s="11"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="11"/>
+      <c r="D62" s="12"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>